<commit_message>
Method add document to a separate class
</commit_message>
<xml_diff>
--- a/courses/3course.xlsx
+++ b/courses/3course.xlsx
@@ -1,18 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24334"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ernest\IdeaProjects\TelegramJavaBot\courses\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\emuratov\IdeaProjects\TelegramJavaBot\courses\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C38EB26-928C-4D46-B218-A5BECA362621}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="135" yWindow="30" windowWidth="20370" windowHeight="10770" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Группа А-1-24" sheetId="1" r:id="rId1"/>
+    <sheet name="А-1-24" sheetId="1" r:id="rId1"/>
     <sheet name="Группа А-2-24" sheetId="2" r:id="rId2"/>
     <sheet name="Группа Ю-2-24" sheetId="3" r:id="rId3"/>
   </sheets>
@@ -21,14 +22,8 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
+    <ext xmlns:xlwcv="http://schemas.microsoft.com/office/spreadsheetml/2024/workbookCompatibilityVersion" uri="{D14903EA-33C4-47F7-8F05-3474C54BE107}">
+      <xlwcv:version setVersion="1"/>
     </ext>
   </extLst>
 </workbook>
@@ -91,7 +86,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -162,9 +157,6 @@
   <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -172,6 +164,9 @@
     <xf numFmtId="20" fontId="2" fillId="2" borderId="1" xfId="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -487,10 +482,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
@@ -505,110 +500,110 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="3"/>
-      <c r="B2" s="4" t="s">
+      <c r="A2" s="2"/>
+      <c r="B2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="3" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="5">
+      <c r="A3" s="4">
         <v>0.33333333333333331</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="F3" s="5" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="5">
+      <c r="A4" s="4">
         <v>0.39583333333333331</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E4" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="F4" s="6" t="s">
+      <c r="F4" s="5" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="5">
+      <c r="A5" s="4">
         <v>0.45833333333333298</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="E5" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="F5" s="6" t="s">
+      <c r="F5" s="5" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="5">
+      <c r="A6" s="4">
         <v>0.52083333333333304</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="D6" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="E6" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="F6" s="6" t="s">
+      <c r="F6" s="5" t="s">
         <v>16</v>
       </c>
     </row>
@@ -629,10 +624,10 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
@@ -647,110 +642,110 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="3"/>
-      <c r="B2" s="4" t="s">
+      <c r="A2" s="2"/>
+      <c r="B2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="3" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="5">
+      <c r="A3" s="4">
         <v>0.33333333333333331</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="F3" s="5" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="5">
+      <c r="A4" s="4">
         <v>0.39583333333333331</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E4" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="F4" s="6" t="s">
+      <c r="F4" s="5" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="5">
+      <c r="A5" s="4">
         <v>0.45833333333333298</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="E5" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="F5" s="6" t="s">
+      <c r="F5" s="5" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="5">
+      <c r="A6" s="4">
         <v>0.52083333333333304</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="D6" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="E6" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="F6" s="6" t="s">
+      <c r="F6" s="5" t="s">
         <v>12</v>
       </c>
     </row>
@@ -769,7 +764,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>